<commit_message>
fixed CPU board in library
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simmers\Documents\GitHub\g5-pcb\STM32F407 era\Traction control modul\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\g5-pcb\STM32F407 era\Traction control modul\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>A</t>
   </si>
@@ -188,16 +188,22 @@
     <t>B&amp;C GND</t>
   </si>
   <si>
-    <t>Fuel</t>
-  </si>
-  <si>
-    <t>fuel</t>
-  </si>
-  <si>
     <t>Connector</t>
   </si>
   <si>
     <t>brake p</t>
+  </si>
+  <si>
+    <t>Fuel GND</t>
+  </si>
+  <si>
+    <t>Fuel 12V</t>
+  </si>
+  <si>
+    <t>Fuel rec</t>
+  </si>
+  <si>
+    <t>Fuel send</t>
   </si>
 </sst>
 </file>
@@ -655,7 +661,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M8"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,15 +675,15 @@
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -766,7 +772,7 @@
         <v>42</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>41</v>
@@ -845,10 +851,10 @@
         <v>46</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>27</v>
@@ -886,10 +892,10 @@
         <v>39</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
added CAN bus connections to TC board
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/pinout.xlsx
@@ -98,12 +98,6 @@
     <t>Travel 2 3.3V</t>
   </si>
   <si>
-    <t>Travel 1 3,3V</t>
-  </si>
-  <si>
-    <t>Travel 3 3.3V</t>
-  </si>
-  <si>
     <t>Travel 4 3.3V</t>
   </si>
   <si>
@@ -204,6 +198,12 @@
   </si>
   <si>
     <t>Fuel send</t>
+  </si>
+  <si>
+    <t>CAN High</t>
+  </si>
+  <si>
+    <t>CAN Low</t>
   </si>
 </sst>
 </file>
@@ -661,7 +661,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -748,7 +748,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>19</v>
@@ -757,28 +757,28 @@
         <v>23</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>12</v>
@@ -792,28 +792,28 @@
         <v>15</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>24</v>
+      <c r="E4" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="4"/>
@@ -830,37 +830,37 @@
         <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="M5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -871,31 +871,31 @@
         <v>17</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="J6" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>13</v>
@@ -908,13 +908,13 @@
     <row r="8" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="12"/>
       <c r="B8" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="22" t="s">
         <v>34</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>36</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>

</xml_diff>

<commit_message>
more final board prepping for production
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/pinout.xlsx
+++ b/STM32F407 era/Traction control modul/pinout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\g5-pcb\STM32F407 era\Traction control modul\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simmers\Documents\GitHub\g5-pcb\STM32F407 era\Traction control modul\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>A</t>
   </si>
@@ -204,13 +204,28 @@
   </si>
   <si>
     <t>CAN Low</t>
+  </si>
+  <si>
+    <t>DirBSense</t>
+  </si>
+  <si>
+    <t>DirASense</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>ECU 1</t>
+  </si>
+  <si>
+    <t>ECU2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +260,12 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -359,7 +380,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -378,6 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,7 +682,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,100 +696,100 @@
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="3" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>40</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -784,76 +805,82 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+    <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5"/>
+      <c r="K4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>62</v>
+      </c>
       <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+    <row r="5" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>44</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>54</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -864,28 +891,28 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>46</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -894,114 +921,114 @@
       <c r="J6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
     </row>
     <row r="25" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>